<commit_message>
refined experiment 4 csv
</commit_message>
<xml_diff>
--- a/Experiment 4/experiment4-HillClimbing.xlsx
+++ b/Experiment 4/experiment4-HillClimbing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UPC\Cinquè any\IA\Practicas\IA-Gasolina\Experiment 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lator\Documents\GitHub\IA-Gasolina\Experiment 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFD406D-5606-43DB-97DE-4104BEF9B2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566B16CB-ED89-4311-B64A-7FB3C5164B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="195" windowWidth="21600" windowHeight="11385" xr2:uid="{3A114B70-8D78-4423-BD01-93E493EDDFC2}"/>
+    <workbookView xWindow="34410" yWindow="4710" windowWidth="16913" windowHeight="8498" xr2:uid="{3A114B70-8D78-4423-BD01-93E493EDDFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="17">
   <si>
     <t>Nombre Gasolineres</t>
   </si>
@@ -50,6 +52,39 @@
   </si>
   <si>
     <t>mitjana temps</t>
+  </si>
+  <si>
+    <t>Hill Climbing</t>
+  </si>
+  <si>
+    <t>Simulated Annealing</t>
+  </si>
+  <si>
+    <t>Simulated Annealing pero:   steps: 20000   i stiter: 20000</t>
+  </si>
+  <si>
+    <t>Hill climbing vs default annealing</t>
+  </si>
+  <si>
+    <t>Tipus</t>
+  </si>
+  <si>
+    <t>temps execucio</t>
+  </si>
+  <si>
+    <t>Hill climbing</t>
+  </si>
+  <si>
+    <t>S annealing</t>
+  </si>
+  <si>
+    <t>S annealing default vs Annealing (20000)</t>
+  </si>
+  <si>
+    <t>Param. Experiment 3</t>
+  </si>
+  <si>
+    <t>Steps i stiter: 20.000</t>
   </si>
 </sst>
 </file>
@@ -57,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -90,7 +125,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -109,7 +144,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -405,207 +440,1062 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F93638D-2B3F-4F78-BC0A-FD749422560B}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>0.56253790000000004</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>0.56024030000000002</v>
       </c>
-      <c r="E2">
-        <f>AVERAGE(C2,D2)</f>
+      <c r="E3">
+        <f>AVERAGE(C3,D3)</f>
         <v>0.56138909999999997</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>97318</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>200</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>6.0889009999999999</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>6.1535992999999998</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E9" si="0">AVERAGE(C3,D3)</f>
+      <c r="E4">
+        <f t="shared" ref="E4:E10" si="0">AVERAGE(C4,D4)</f>
         <v>6.1212501499999998</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>197452</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>30</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>300</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>29.6675386</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>31.8801302</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>30.773834399999998</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>296804</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>40</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>400</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>91.697169000000002</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>98.457334299999999</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>95.077251649999994</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>396346</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>50</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>500</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>227.014062</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>232.73485429999999</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>229.87445815000001</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>496618</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>60</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>600</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>551.88312699999994</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>568.64734380000004</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>560.26523539999994</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>595886</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>70</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>700</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>1173.2399286</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>1203.9319539000001</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>1188.5859412499999</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>695636</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>80</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>800</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2162.8157612</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>2192.0391169999998</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>2177.4274390999999</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>794120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>0.1883348</v>
+      </c>
+      <c r="D14">
+        <v>83806</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>200</v>
+      </c>
+      <c r="C15">
+        <v>0.44733299999999998</v>
+      </c>
+      <c r="D15">
+        <v>164374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>300</v>
+      </c>
+      <c r="C16">
+        <v>0.85606990000000005</v>
+      </c>
+      <c r="D16">
+        <v>254758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>400</v>
+      </c>
+      <c r="C17">
+        <v>1.3075311000000001</v>
+      </c>
+      <c r="D17">
+        <v>326608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>50</v>
+      </c>
+      <c r="B18">
+        <v>500</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.9486346000000001</v>
+      </c>
+      <c r="D18">
+        <v>417264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>60</v>
+      </c>
+      <c r="B19">
+        <v>600</v>
+      </c>
+      <c r="C19">
+        <v>2.6807159</v>
+      </c>
+      <c r="D19">
+        <v>497286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>70</v>
+      </c>
+      <c r="B20">
+        <v>700</v>
+      </c>
+      <c r="C20">
+        <v>3.6049528999999998</v>
+      </c>
+      <c r="D20">
+        <v>580638</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>80</v>
+      </c>
+      <c r="B21">
+        <v>800</v>
+      </c>
+      <c r="C21">
+        <v>4.6428234000000002</v>
+      </c>
+      <c r="D21">
+        <v>655610</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>0.51750589999999996</v>
+      </c>
+      <c r="D26">
+        <v>82412</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>200</v>
+      </c>
+      <c r="C27">
+        <v>1.6480881999999999</v>
+      </c>
+      <c r="D27">
+        <v>167476</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>300</v>
+      </c>
+      <c r="C28">
+        <v>3.3093509999999999</v>
+      </c>
+      <c r="D28">
+        <v>253046</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>400</v>
+      </c>
+      <c r="C29">
+        <v>5.6877161000000003</v>
+      </c>
+      <c r="D29">
+        <v>327468</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>50</v>
+      </c>
+      <c r="B30">
+        <v>500</v>
+      </c>
+      <c r="C30" s="1">
+        <v>8.7923535000000008</v>
+      </c>
+      <c r="D30">
+        <v>427258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>60</v>
+      </c>
+      <c r="B31">
+        <v>600</v>
+      </c>
+      <c r="C31">
+        <v>12.564935800000001</v>
+      </c>
+      <c r="D31">
+        <v>504802</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>70</v>
+      </c>
+      <c r="B32">
+        <v>700</v>
+      </c>
+      <c r="C32">
+        <v>16.469736099999999</v>
+      </c>
+      <c r="D32">
+        <v>588902</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>80</v>
+      </c>
+      <c r="B33">
+        <v>800</v>
+      </c>
+      <c r="C33">
+        <v>21.488606300000001</v>
+      </c>
+      <c r="D33">
+        <v>665466</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>100</v>
+      </c>
+      <c r="D40">
+        <v>0.56138909999999997</v>
+      </c>
+      <c r="E40">
+        <v>97318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>200</v>
+      </c>
+      <c r="D41">
+        <v>6.1212501499999998</v>
+      </c>
+      <c r="E41">
+        <v>197452</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42">
+        <v>300</v>
+      </c>
+      <c r="D42">
+        <v>30.773834399999998</v>
+      </c>
+      <c r="E42">
+        <v>296804</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="C43">
+        <v>400</v>
+      </c>
+      <c r="D43">
+        <v>95.077251649999994</v>
+      </c>
+      <c r="E43">
+        <v>396346</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <v>50</v>
+      </c>
+      <c r="C44">
+        <v>500</v>
+      </c>
+      <c r="D44">
+        <v>229.87445815000001</v>
+      </c>
+      <c r="E44">
+        <v>496618</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>60</v>
+      </c>
+      <c r="C45">
+        <v>600</v>
+      </c>
+      <c r="D45">
+        <v>560.26523539999994</v>
+      </c>
+      <c r="E45">
+        <v>595886</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>70</v>
+      </c>
+      <c r="C46">
+        <v>700</v>
+      </c>
+      <c r="D46">
+        <v>1188.5859412499999</v>
+      </c>
+      <c r="E46">
+        <v>695636</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>80</v>
+      </c>
+      <c r="C47">
+        <v>800</v>
+      </c>
+      <c r="D47">
+        <v>2177.4274390999999</v>
+      </c>
+      <c r="E47">
+        <v>794120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>100</v>
+      </c>
+      <c r="D48">
+        <v>0.1883348</v>
+      </c>
+      <c r="E48">
+        <v>83806</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>20</v>
+      </c>
+      <c r="C49">
+        <v>200</v>
+      </c>
+      <c r="D49">
+        <v>0.44733299999999998</v>
+      </c>
+      <c r="E49">
+        <v>164374</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50">
+        <v>30</v>
+      </c>
+      <c r="C50">
+        <v>300</v>
+      </c>
+      <c r="D50">
+        <v>0.85606990000000005</v>
+      </c>
+      <c r="E50">
+        <v>254758</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51">
+        <v>40</v>
+      </c>
+      <c r="C51">
+        <v>400</v>
+      </c>
+      <c r="D51">
+        <v>1.3075311000000001</v>
+      </c>
+      <c r="E51">
+        <v>326608</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52">
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <v>500</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1.9486346000000001</v>
+      </c>
+      <c r="E52">
+        <v>417264</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53">
+        <v>60</v>
+      </c>
+      <c r="C53">
+        <v>600</v>
+      </c>
+      <c r="D53">
+        <v>2.6807159</v>
+      </c>
+      <c r="E53">
+        <v>497286</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54">
+        <v>70</v>
+      </c>
+      <c r="C54">
+        <v>700</v>
+      </c>
+      <c r="D54">
+        <v>3.6049528999999998</v>
+      </c>
+      <c r="E54">
+        <v>580638</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55">
+        <v>80</v>
+      </c>
+      <c r="C55">
+        <v>800</v>
+      </c>
+      <c r="D55">
+        <v>4.6428234000000002</v>
+      </c>
+      <c r="E55">
+        <v>655610</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62">
+        <v>10</v>
+      </c>
+      <c r="C62">
+        <v>100</v>
+      </c>
+      <c r="D62">
+        <v>0.1883348</v>
+      </c>
+      <c r="E62">
+        <v>83806</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63">
+        <v>20</v>
+      </c>
+      <c r="C63">
+        <v>200</v>
+      </c>
+      <c r="D63">
+        <v>0.44733299999999998</v>
+      </c>
+      <c r="E63">
+        <v>164374</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64">
+        <v>30</v>
+      </c>
+      <c r="C64">
+        <v>300</v>
+      </c>
+      <c r="D64">
+        <v>0.85606990000000005</v>
+      </c>
+      <c r="E64">
+        <v>254758</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65">
+        <v>40</v>
+      </c>
+      <c r="C65">
+        <v>400</v>
+      </c>
+      <c r="D65">
+        <v>1.3075311000000001</v>
+      </c>
+      <c r="E65">
+        <v>326608</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <v>500</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1.9486346000000001</v>
+      </c>
+      <c r="E66">
+        <v>417264</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67">
+        <v>60</v>
+      </c>
+      <c r="C67">
+        <v>600</v>
+      </c>
+      <c r="D67">
+        <v>2.6807159</v>
+      </c>
+      <c r="E67">
+        <v>497286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68">
+        <v>70</v>
+      </c>
+      <c r="C68">
+        <v>700</v>
+      </c>
+      <c r="D68">
+        <v>3.6049528999999998</v>
+      </c>
+      <c r="E68">
+        <v>580638</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69">
+        <v>80</v>
+      </c>
+      <c r="C69">
+        <v>800</v>
+      </c>
+      <c r="D69">
+        <v>4.6428234000000002</v>
+      </c>
+      <c r="E69">
+        <v>655610</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70">
+        <v>10</v>
+      </c>
+      <c r="C70">
+        <v>100</v>
+      </c>
+      <c r="D70">
+        <v>0.51750589999999996</v>
+      </c>
+      <c r="E70">
+        <v>82412</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71">
+        <v>20</v>
+      </c>
+      <c r="C71">
+        <v>200</v>
+      </c>
+      <c r="D71">
+        <v>1.6480881999999999</v>
+      </c>
+      <c r="E71">
+        <v>167476</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72">
+        <v>30</v>
+      </c>
+      <c r="C72">
+        <v>300</v>
+      </c>
+      <c r="D72">
+        <v>3.3093509999999999</v>
+      </c>
+      <c r="E72">
+        <v>253046</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73">
+        <v>40</v>
+      </c>
+      <c r="C73">
+        <v>400</v>
+      </c>
+      <c r="D73">
+        <v>5.6877161000000003</v>
+      </c>
+      <c r="E73">
+        <v>327468</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74">
+        <v>50</v>
+      </c>
+      <c r="C74">
+        <v>500</v>
+      </c>
+      <c r="D74" s="1">
+        <v>8.7923535000000008</v>
+      </c>
+      <c r="E74">
+        <v>427258</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75">
+        <v>60</v>
+      </c>
+      <c r="C75">
+        <v>600</v>
+      </c>
+      <c r="D75">
+        <v>12.564935800000001</v>
+      </c>
+      <c r="E75">
+        <v>504802</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76">
+        <v>70</v>
+      </c>
+      <c r="C76">
+        <v>700</v>
+      </c>
+      <c r="D76">
+        <v>16.469736099999999</v>
+      </c>
+      <c r="E76">
+        <v>588902</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>16</v>
+      </c>
+      <c r="B77">
+        <v>80</v>
+      </c>
+      <c r="C77">
+        <v>800</v>
+      </c>
+      <c r="D77">
+        <v>21.488606300000001</v>
+      </c>
+      <c r="E77">
+        <v>665466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>